<commit_message>
Excel Export and SVG design done
</commit_message>
<xml_diff>
--- a/assets/data/DataBase.xlsx
+++ b/assets/data/DataBase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,14 +1223,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1426,15 +1426,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>